<commit_message>
Paper submitted - Neurocomputing
</commit_message>
<xml_diff>
--- a/data/processed/df_metanalysis.xlsx
+++ b/data/processed/df_metanalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dameliotomas\review-emotion-recognition-eda\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F00A1C-A288-4498-9972-2A9F1A3833CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB20F20-63BF-402C-946F-597B4DC5815C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -220,9 +220,6 @@
     <t>class_Extreme Learning Machine (ELM) Without Baseline Compensation Baseline Compensated</t>
   </si>
   <si>
-    <t>Other / Unclear</t>
-  </si>
-  <si>
     <t>180-2</t>
   </si>
   <si>
@@ -647,6 +644,9 @@
   </si>
   <si>
     <t>Elalamy, R., Fanourakis, M., &amp; Chanel, G. (2021, September). Multi-modal emotion recognition using recurrence plots and transfer learning on physiological signals. In 2021 9th International Conference on Affective Computing and Intelligent Interaction (ACII) (pp. 1-7). IEEE.</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -1011,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97:XFD98"/>
+    <sheetView tabSelected="1" topLeftCell="C23" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1891,7 +1891,7 @@
         <v>61.72</v>
       </c>
       <c r="L23" t="s">
-        <v>66</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.45">
@@ -1899,7 +1899,7 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C24" t="s">
         <v>63</v>
@@ -1911,7 +1911,7 @@
         <v>64</v>
       </c>
       <c r="F24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G24">
         <v>40</v>
@@ -1929,7 +1929,7 @@
         <v>64.84</v>
       </c>
       <c r="L24" t="s">
-        <v>66</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.45">
@@ -1940,7 +1940,7 @@
         <v>245</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D25">
         <v>2017</v>
@@ -1949,7 +1949,7 @@
         <v>25</v>
       </c>
       <c r="F25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G25">
         <v>32</v>
@@ -1978,7 +1978,7 @@
         <v>242</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D26">
         <v>2017</v>
@@ -1987,7 +1987,7 @@
         <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G26">
         <v>32</v>
@@ -2005,7 +2005,7 @@
         <v>60.54</v>
       </c>
       <c r="L26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.45">
@@ -2016,7 +2016,7 @@
         <v>243</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27">
         <v>2017</v>
@@ -2025,7 +2025,7 @@
         <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G27">
         <v>32</v>
@@ -2054,7 +2054,7 @@
         <v>244</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D28">
         <v>2017</v>
@@ -2063,7 +2063,7 @@
         <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G28">
         <v>32</v>
@@ -2089,10 +2089,10 @@
         <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D29">
         <v>2017</v>
@@ -2101,7 +2101,7 @@
         <v>25</v>
       </c>
       <c r="F29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G29">
         <v>32</v>
@@ -2119,7 +2119,7 @@
         <v>71.040000000000006</v>
       </c>
       <c r="L29" t="s">
-        <v>66</v>
+        <v>208</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.45">
@@ -2127,10 +2127,10 @@
         <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D30">
         <v>2017</v>
@@ -2139,7 +2139,7 @@
         <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G30">
         <v>32</v>
@@ -2157,7 +2157,7 @@
         <v>89.29</v>
       </c>
       <c r="L30" t="s">
-        <v>66</v>
+        <v>208</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.45">
@@ -2165,10 +2165,10 @@
         <v>63</v>
       </c>
       <c r="B31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" t="s">
         <v>78</v>
-      </c>
-      <c r="C31" t="s">
-        <v>79</v>
       </c>
       <c r="D31">
         <v>2019</v>
@@ -2177,7 +2177,7 @@
         <v>25</v>
       </c>
       <c r="F31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G31">
         <v>32</v>
@@ -2195,7 +2195,7 @@
         <v>62.4</v>
       </c>
       <c r="L31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.45">
@@ -2203,10 +2203,10 @@
         <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D32">
         <v>2019</v>
@@ -2215,7 +2215,7 @@
         <v>25</v>
       </c>
       <c r="F32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G32">
         <v>32</v>
@@ -2233,7 +2233,7 @@
         <v>61.6</v>
       </c>
       <c r="L32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.45">
@@ -2241,10 +2241,10 @@
         <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D33">
         <v>2019</v>
@@ -2253,7 +2253,7 @@
         <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G33">
         <v>32</v>
@@ -2271,7 +2271,7 @@
         <v>67.2</v>
       </c>
       <c r="L33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.45">
@@ -2279,10 +2279,10 @@
         <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D34">
         <v>2019</v>
@@ -2291,7 +2291,7 @@
         <v>25</v>
       </c>
       <c r="F34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G34">
         <v>32</v>
@@ -2309,7 +2309,7 @@
         <v>61.8</v>
       </c>
       <c r="L34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.45">
@@ -2317,10 +2317,10 @@
         <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D35">
         <v>2019</v>
@@ -2329,7 +2329,7 @@
         <v>25</v>
       </c>
       <c r="F35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G35">
         <v>32</v>
@@ -2347,7 +2347,7 @@
         <v>68.5</v>
       </c>
       <c r="L35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.45">
@@ -2355,10 +2355,10 @@
         <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D36">
         <v>2019</v>
@@ -2367,7 +2367,7 @@
         <v>25</v>
       </c>
       <c r="F36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G36">
         <v>32</v>
@@ -2385,7 +2385,7 @@
         <v>69.8</v>
       </c>
       <c r="L36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.45">
@@ -2393,10 +2393,10 @@
         <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D37">
         <v>2019</v>
@@ -2405,7 +2405,7 @@
         <v>25</v>
       </c>
       <c r="F37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G37">
         <v>32</v>
@@ -2423,7 +2423,7 @@
         <v>61.8</v>
       </c>
       <c r="L37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.45">
@@ -2431,10 +2431,10 @@
         <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D38">
         <v>2019</v>
@@ -2443,7 +2443,7 @@
         <v>25</v>
       </c>
       <c r="F38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G38">
         <v>32</v>
@@ -2461,7 +2461,7 @@
         <v>59.8</v>
       </c>
       <c r="L38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.45">
@@ -2469,10 +2469,10 @@
         <v>63</v>
       </c>
       <c r="B39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D39">
         <v>2019</v>
@@ -2481,7 +2481,7 @@
         <v>25</v>
       </c>
       <c r="F39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G39">
         <v>32</v>
@@ -2499,7 +2499,7 @@
         <v>64.900000000000006</v>
       </c>
       <c r="L39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.45">
@@ -2507,10 +2507,10 @@
         <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D40">
         <v>2019</v>
@@ -2519,7 +2519,7 @@
         <v>25</v>
       </c>
       <c r="F40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G40">
         <v>32</v>
@@ -2537,7 +2537,7 @@
         <v>60.5</v>
       </c>
       <c r="L40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.45">
@@ -2545,10 +2545,10 @@
         <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D41">
         <v>2019</v>
@@ -2557,7 +2557,7 @@
         <v>25</v>
       </c>
       <c r="F41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G41">
         <v>32</v>
@@ -2575,7 +2575,7 @@
         <v>65.8</v>
       </c>
       <c r="L41" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.45">
@@ -2583,10 +2583,10 @@
         <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D42">
         <v>2019</v>
@@ -2595,7 +2595,7 @@
         <v>25</v>
       </c>
       <c r="F42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G42">
         <v>32</v>
@@ -2613,7 +2613,7 @@
         <v>66.7</v>
       </c>
       <c r="L42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.45">
@@ -2624,7 +2624,7 @@
         <v>353</v>
       </c>
       <c r="C43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D43">
         <v>2020</v>
@@ -2633,7 +2633,7 @@
         <v>25</v>
       </c>
       <c r="F43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G43">
         <v>32</v>
@@ -2662,7 +2662,7 @@
         <v>355</v>
       </c>
       <c r="C44" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D44">
         <v>2020</v>
@@ -2671,7 +2671,7 @@
         <v>25</v>
       </c>
       <c r="F44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G44">
         <v>32</v>
@@ -2689,7 +2689,7 @@
         <v>52.7</v>
       </c>
       <c r="L44" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.45">
@@ -2700,7 +2700,7 @@
         <v>354</v>
       </c>
       <c r="C45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D45">
         <v>2020</v>
@@ -2709,7 +2709,7 @@
         <v>25</v>
       </c>
       <c r="F45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G45">
         <v>32</v>
@@ -2738,7 +2738,7 @@
         <v>351</v>
       </c>
       <c r="C46" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D46">
         <v>2020</v>
@@ -2747,7 +2747,7 @@
         <v>25</v>
       </c>
       <c r="F46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G46">
         <v>32</v>
@@ -2765,7 +2765,7 @@
         <v>72</v>
       </c>
       <c r="L46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.45">
@@ -2776,7 +2776,7 @@
         <v>356</v>
       </c>
       <c r="C47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D47">
         <v>2020</v>
@@ -2785,7 +2785,7 @@
         <v>25</v>
       </c>
       <c r="F47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G47">
         <v>32</v>
@@ -2803,7 +2803,7 @@
         <v>50.8</v>
       </c>
       <c r="L47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.45">
@@ -2811,10 +2811,10 @@
         <v>66</v>
       </c>
       <c r="B48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D48">
         <v>2020</v>
@@ -2823,7 +2823,7 @@
         <v>25</v>
       </c>
       <c r="F48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G48">
         <v>32</v>
@@ -2849,10 +2849,10 @@
         <v>66</v>
       </c>
       <c r="B49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C49" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D49">
         <v>2020</v>
@@ -2861,7 +2861,7 @@
         <v>25</v>
       </c>
       <c r="F49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G49">
         <v>32</v>
@@ -2887,10 +2887,10 @@
         <v>66</v>
       </c>
       <c r="B50" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C50" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D50">
         <v>2020</v>
@@ -2899,7 +2899,7 @@
         <v>25</v>
       </c>
       <c r="F50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G50">
         <v>32</v>
@@ -2925,10 +2925,10 @@
         <v>66</v>
       </c>
       <c r="B51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C51" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D51">
         <v>2020</v>
@@ -2937,7 +2937,7 @@
         <v>25</v>
       </c>
       <c r="F51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G51">
         <v>32</v>
@@ -2955,7 +2955,7 @@
         <v>50.54</v>
       </c>
       <c r="L51" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.45">
@@ -2966,7 +2966,7 @@
         <v>381</v>
       </c>
       <c r="C52" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D52">
         <v>2019</v>
@@ -2975,7 +2975,7 @@
         <v>64</v>
       </c>
       <c r="F52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G52">
         <v>40</v>
@@ -3004,7 +3004,7 @@
         <v>380</v>
       </c>
       <c r="C53" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D53">
         <v>2019</v>
@@ -3013,7 +3013,7 @@
         <v>64</v>
       </c>
       <c r="F53" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G53">
         <v>40</v>
@@ -3031,7 +3031,7 @@
         <v>53.8</v>
       </c>
       <c r="L53" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.45">
@@ -3042,7 +3042,7 @@
         <v>383</v>
       </c>
       <c r="C54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D54">
         <v>2019</v>
@@ -3051,7 +3051,7 @@
         <v>64</v>
       </c>
       <c r="F54" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G54">
         <v>40</v>
@@ -3069,7 +3069,7 @@
         <v>82.2</v>
       </c>
       <c r="L54" t="s">
-        <v>66</v>
+        <v>208</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.45">
@@ -3080,7 +3080,7 @@
         <v>382</v>
       </c>
       <c r="C55" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D55">
         <v>2019</v>
@@ -3089,7 +3089,7 @@
         <v>64</v>
       </c>
       <c r="F55" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G55">
         <v>40</v>
@@ -3107,7 +3107,7 @@
         <v>77.599999999999994</v>
       </c>
       <c r="L55" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.45">
@@ -3115,10 +3115,10 @@
         <v>82</v>
       </c>
       <c r="B56" t="s">
+        <v>117</v>
+      </c>
+      <c r="C56" t="s">
         <v>118</v>
-      </c>
-      <c r="C56" t="s">
-        <v>119</v>
       </c>
       <c r="D56">
         <v>2019</v>
@@ -3127,7 +3127,7 @@
         <v>64</v>
       </c>
       <c r="F56" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G56">
         <v>40</v>
@@ -3145,7 +3145,7 @@
         <v>69</v>
       </c>
       <c r="L56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.45">
@@ -3153,10 +3153,10 @@
         <v>82</v>
       </c>
       <c r="B57" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C57" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D57">
         <v>2019</v>
@@ -3165,7 +3165,7 @@
         <v>64</v>
       </c>
       <c r="F57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G57">
         <v>40</v>
@@ -3183,7 +3183,7 @@
         <v>64</v>
       </c>
       <c r="L57" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.45">
@@ -3191,10 +3191,10 @@
         <v>82</v>
       </c>
       <c r="B58" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C58" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D58">
         <v>2019</v>
@@ -3203,7 +3203,7 @@
         <v>64</v>
       </c>
       <c r="F58" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G58">
         <v>40</v>
@@ -3229,10 +3229,10 @@
         <v>82</v>
       </c>
       <c r="B59" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C59" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D59">
         <v>2019</v>
@@ -3241,7 +3241,7 @@
         <v>64</v>
       </c>
       <c r="F59" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G59">
         <v>40</v>
@@ -3259,7 +3259,7 @@
         <v>64</v>
       </c>
       <c r="L59" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.45">
@@ -3267,10 +3267,10 @@
         <v>82</v>
       </c>
       <c r="B60" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C60" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D60">
         <v>2019</v>
@@ -3279,7 +3279,7 @@
         <v>64</v>
       </c>
       <c r="F60" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G60">
         <v>40</v>
@@ -3297,7 +3297,7 @@
         <v>66</v>
       </c>
       <c r="L60" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.45">
@@ -3305,10 +3305,10 @@
         <v>82</v>
       </c>
       <c r="B61" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C61" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D61">
         <v>2019</v>
@@ -3317,7 +3317,7 @@
         <v>64</v>
       </c>
       <c r="F61" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G61">
         <v>40</v>
@@ -3343,10 +3343,10 @@
         <v>82</v>
       </c>
       <c r="B62" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C62" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D62">
         <v>2019</v>
@@ -3355,7 +3355,7 @@
         <v>64</v>
       </c>
       <c r="F62" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G62">
         <v>40</v>
@@ -3373,7 +3373,7 @@
         <v>75</v>
       </c>
       <c r="L62" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.45">
@@ -3384,7 +3384,7 @@
         <v>460</v>
       </c>
       <c r="C63" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D63">
         <v>2020</v>
@@ -3393,7 +3393,7 @@
         <v>25</v>
       </c>
       <c r="F63" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G63">
         <v>32</v>
@@ -3411,7 +3411,7 @@
         <v>68.900000000000006</v>
       </c>
       <c r="L63" t="s">
-        <v>66</v>
+        <v>208</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.45">
@@ -3422,16 +3422,16 @@
         <v>470</v>
       </c>
       <c r="C64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D64">
         <v>2020</v>
       </c>
       <c r="E64" t="s">
+        <v>131</v>
+      </c>
+      <c r="F64" t="s">
         <v>132</v>
-      </c>
-      <c r="F64" t="s">
-        <v>133</v>
       </c>
       <c r="G64">
         <v>457</v>
@@ -3449,7 +3449,7 @@
         <v>59.78</v>
       </c>
       <c r="L64" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.45">
@@ -3460,16 +3460,16 @@
         <v>471</v>
       </c>
       <c r="C65" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D65">
         <v>2020</v>
       </c>
       <c r="E65" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F65" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G65">
         <v>457</v>
@@ -3487,7 +3487,7 @@
         <v>60</v>
       </c>
       <c r="L65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.45">
@@ -3498,16 +3498,16 @@
         <v>472</v>
       </c>
       <c r="C66" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D66">
         <v>2020</v>
       </c>
       <c r="E66" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F66" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G66">
         <v>457</v>
@@ -3525,7 +3525,7 @@
         <v>60.47</v>
       </c>
       <c r="L66" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.45">
@@ -3536,16 +3536,16 @@
         <v>473</v>
       </c>
       <c r="C67" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D67">
         <v>2020</v>
       </c>
       <c r="E67" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F67" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G67">
         <v>457</v>
@@ -3563,7 +3563,7 @@
         <v>60.66</v>
       </c>
       <c r="L67" t="s">
-        <v>66</v>
+        <v>208</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.45">
@@ -3574,16 +3574,16 @@
         <v>474</v>
       </c>
       <c r="C68" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D68">
         <v>2020</v>
       </c>
       <c r="E68" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F68" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G68">
         <v>457</v>
@@ -3601,7 +3601,7 @@
         <v>60</v>
       </c>
       <c r="L68" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.45">
@@ -3612,16 +3612,16 @@
         <v>480</v>
       </c>
       <c r="C69" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D69">
         <v>2019</v>
       </c>
       <c r="E69" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F69" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G69">
         <v>457</v>
@@ -3639,7 +3639,7 @@
         <v>55.92</v>
       </c>
       <c r="L69" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.45">
@@ -3647,10 +3647,10 @@
         <v>97</v>
       </c>
       <c r="B70" t="s">
+        <v>139</v>
+      </c>
+      <c r="C70" t="s">
         <v>140</v>
-      </c>
-      <c r="C70" t="s">
-        <v>141</v>
       </c>
       <c r="D70">
         <v>2020</v>
@@ -3659,7 +3659,7 @@
         <v>25</v>
       </c>
       <c r="F70" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G70">
         <v>32</v>
@@ -3677,7 +3677,7 @@
         <v>68.75</v>
       </c>
       <c r="L70" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.45">
@@ -3685,10 +3685,10 @@
         <v>97</v>
       </c>
       <c r="B71" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C71" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D71">
         <v>2020</v>
@@ -3697,7 +3697,7 @@
         <v>25</v>
       </c>
       <c r="F71" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G71">
         <v>32</v>
@@ -3715,7 +3715,7 @@
         <v>50.24</v>
       </c>
       <c r="L71" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.45">
@@ -3723,10 +3723,10 @@
         <v>97</v>
       </c>
       <c r="B72" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C72" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D72">
         <v>2020</v>
@@ -3735,7 +3735,7 @@
         <v>25</v>
       </c>
       <c r="F72" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G72">
         <v>32</v>
@@ -3753,7 +3753,7 @@
         <v>71.430000000000007</v>
       </c>
       <c r="L72" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.45">
@@ -3761,10 +3761,10 @@
         <v>97</v>
       </c>
       <c r="B73" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C73" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D73">
         <v>2020</v>
@@ -3773,7 +3773,7 @@
         <v>25</v>
       </c>
       <c r="F73" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G73">
         <v>32</v>
@@ -3791,7 +3791,7 @@
         <v>59.38</v>
       </c>
       <c r="L73" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.45">
@@ -3799,10 +3799,10 @@
         <v>97</v>
       </c>
       <c r="B74" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C74" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D74">
         <v>2020</v>
@@ -3811,7 +3811,7 @@
         <v>25</v>
       </c>
       <c r="F74" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G74">
         <v>32</v>
@@ -3829,7 +3829,7 @@
         <v>50</v>
       </c>
       <c r="L74" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.45">
@@ -3837,10 +3837,10 @@
         <v>97</v>
       </c>
       <c r="B75" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C75" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D75">
         <v>2020</v>
@@ -3849,7 +3849,7 @@
         <v>25</v>
       </c>
       <c r="F75" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G75">
         <v>32</v>
@@ -3867,7 +3867,7 @@
         <v>59.38</v>
       </c>
       <c r="L75" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.45">
@@ -3875,10 +3875,10 @@
         <v>97</v>
       </c>
       <c r="B76" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C76" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D76">
         <v>2020</v>
@@ -3887,7 +3887,7 @@
         <v>25</v>
       </c>
       <c r="F76" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G76">
         <v>32</v>
@@ -3905,7 +3905,7 @@
         <v>31.25</v>
       </c>
       <c r="L76" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.45">
@@ -3913,10 +3913,10 @@
         <v>97</v>
       </c>
       <c r="B77" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C77" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D77">
         <v>2020</v>
@@ -3925,7 +3925,7 @@
         <v>25</v>
       </c>
       <c r="F77" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G77">
         <v>32</v>
@@ -3943,7 +3943,7 @@
         <v>40.630000000000003</v>
       </c>
       <c r="L77" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.45">
@@ -3954,7 +3954,7 @@
         <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D78">
         <v>2023</v>
@@ -3963,25 +3963,25 @@
         <v>64</v>
       </c>
       <c r="F78" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G78">
         <v>40</v>
       </c>
       <c r="H78" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I78">
         <v>70.179999999999993</v>
       </c>
       <c r="J78" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K78">
         <v>54.55</v>
       </c>
       <c r="L78" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.45">
@@ -3992,7 +3992,7 @@
         <v>2</v>
       </c>
       <c r="C79" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D79">
         <v>2023</v>
@@ -4001,19 +4001,19 @@
         <v>64</v>
       </c>
       <c r="F79" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G79">
         <v>40</v>
       </c>
       <c r="H79" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I79">
         <v>37.26</v>
       </c>
       <c r="J79" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K79">
         <v>41.37</v>
@@ -4030,7 +4030,7 @@
         <v>3</v>
       </c>
       <c r="C80" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D80">
         <v>2023</v>
@@ -4039,25 +4039,25 @@
         <v>64</v>
       </c>
       <c r="F80" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G80">
         <v>40</v>
       </c>
       <c r="H80" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I80">
         <v>72.75</v>
       </c>
       <c r="J80" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K80">
         <v>61.860000000000007</v>
       </c>
       <c r="L80" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.45">
@@ -4068,7 +4068,7 @@
         <v>4</v>
       </c>
       <c r="C81" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D81">
         <v>2023</v>
@@ -4077,19 +4077,19 @@
         <v>64</v>
       </c>
       <c r="F81" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G81">
         <v>40</v>
       </c>
       <c r="H81" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I81">
         <v>64.510000000000005</v>
       </c>
       <c r="J81" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K81">
         <v>52.459999999999987</v>
@@ -4106,34 +4106,34 @@
         <v>5</v>
       </c>
       <c r="C82" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D82">
         <v>2023</v>
       </c>
       <c r="E82" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F82" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G82">
         <v>40</v>
       </c>
       <c r="H82" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I82">
         <v>69.62</v>
       </c>
       <c r="J82" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K82">
         <v>93.320000000000007</v>
       </c>
       <c r="L82" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.45">
@@ -4144,28 +4144,28 @@
         <v>6</v>
       </c>
       <c r="C83" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D83">
         <v>2023</v>
       </c>
       <c r="E83" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F83" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G83">
         <v>40</v>
       </c>
       <c r="H83" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I83">
         <v>60.48</v>
       </c>
       <c r="J83" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K83">
         <v>70.87</v>
@@ -4182,34 +4182,34 @@
         <v>7</v>
       </c>
       <c r="C84" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D84">
         <v>2023</v>
       </c>
       <c r="E84" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F84" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G84">
         <v>40</v>
       </c>
       <c r="H84" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I84">
         <v>74.48</v>
       </c>
       <c r="J84" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K84">
         <v>84.76</v>
       </c>
       <c r="L84" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.45">
@@ -4220,28 +4220,28 @@
         <v>8</v>
       </c>
       <c r="C85" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D85">
         <v>2023</v>
       </c>
       <c r="E85" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F85" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G85">
         <v>40</v>
       </c>
       <c r="H85" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I85">
         <v>57.65</v>
       </c>
       <c r="J85" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K85">
         <v>77.66</v>
@@ -4258,34 +4258,34 @@
         <v>9</v>
       </c>
       <c r="C86" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D86">
         <v>2023</v>
       </c>
       <c r="E86" t="s">
+        <v>165</v>
+      </c>
+      <c r="F86" t="s">
         <v>166</v>
-      </c>
-      <c r="F86" t="s">
-        <v>167</v>
       </c>
       <c r="G86">
         <v>58</v>
       </c>
       <c r="H86" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I86">
         <v>65.34</v>
       </c>
       <c r="J86" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K86">
         <v>64.849999999999994</v>
       </c>
       <c r="L86" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.45">
@@ -4296,34 +4296,34 @@
         <v>10</v>
       </c>
       <c r="C87" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D87">
         <v>2023</v>
       </c>
       <c r="E87" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F87" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G87">
         <v>58</v>
       </c>
       <c r="H87" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I87">
         <v>45.15</v>
       </c>
       <c r="J87" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K87">
         <v>46.150000000000013</v>
       </c>
       <c r="L87" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.45">
@@ -4334,34 +4334,34 @@
         <v>11</v>
       </c>
       <c r="C88" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D88">
         <v>2023</v>
       </c>
       <c r="E88" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F88" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G88">
         <v>58</v>
       </c>
       <c r="H88" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I88">
         <v>78.959999999999994</v>
       </c>
       <c r="J88" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K88">
         <v>79.52</v>
       </c>
       <c r="L88" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.45">
@@ -4372,7 +4372,7 @@
         <v>12</v>
       </c>
       <c r="C89" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D89">
         <v>2022</v>
@@ -4381,25 +4381,25 @@
         <v>25</v>
       </c>
       <c r="F89" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G89">
         <v>32</v>
       </c>
       <c r="H89" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I89">
         <v>71.64</v>
       </c>
       <c r="J89" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K89">
         <v>70.7</v>
       </c>
       <c r="L89" t="s">
-        <v>66</v>
+        <v>208</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.45">
@@ -4410,7 +4410,7 @@
         <v>13</v>
       </c>
       <c r="C90" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D90">
         <v>2022</v>
@@ -4419,25 +4419,25 @@
         <v>64</v>
       </c>
       <c r="F90" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G90">
         <v>32</v>
       </c>
       <c r="H90" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I90">
         <v>80.94</v>
       </c>
       <c r="J90" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K90">
         <v>80.63</v>
       </c>
       <c r="L90" t="s">
-        <v>66</v>
+        <v>208</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.45">
@@ -4448,7 +4448,7 @@
         <v>14</v>
       </c>
       <c r="C91" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D91">
         <v>2022</v>
@@ -4457,25 +4457,25 @@
         <v>14</v>
       </c>
       <c r="F91" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G91">
         <v>32</v>
       </c>
       <c r="H91" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I91">
         <v>81.84</v>
       </c>
       <c r="J91" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K91">
         <v>78.97999999999999</v>
       </c>
       <c r="L91" t="s">
-        <v>66</v>
+        <v>208</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.45">
@@ -4486,34 +4486,34 @@
         <v>15</v>
       </c>
       <c r="C92" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D92">
         <v>2022</v>
       </c>
       <c r="E92" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F92" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G92">
         <v>32</v>
       </c>
       <c r="H92" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I92">
         <v>63.61</v>
       </c>
       <c r="J92" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K92">
         <v>59.64</v>
       </c>
       <c r="L92" t="s">
-        <v>66</v>
+        <v>208</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.45">
@@ -4524,34 +4524,34 @@
         <v>16</v>
       </c>
       <c r="C93" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D93">
         <v>2022</v>
       </c>
       <c r="E93" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F93" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G93">
         <v>32</v>
       </c>
       <c r="H93" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I93">
         <v>61.02</v>
       </c>
       <c r="J93" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K93">
         <v>58.98</v>
       </c>
       <c r="L93" t="s">
-        <v>66</v>
+        <v>208</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.45">
@@ -4562,34 +4562,34 @@
         <v>17</v>
       </c>
       <c r="C94" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D94">
         <v>2022</v>
       </c>
       <c r="E94" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F94" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G94">
         <v>32</v>
       </c>
       <c r="H94" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I94">
         <v>62.5</v>
       </c>
       <c r="J94" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K94">
         <v>64.959999999999994</v>
       </c>
       <c r="L94" t="s">
-        <v>66</v>
+        <v>208</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.45">
@@ -4600,34 +4600,34 @@
         <v>18</v>
       </c>
       <c r="C95" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D95">
         <v>2022</v>
       </c>
       <c r="E95" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F95" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G95">
         <v>32</v>
       </c>
       <c r="H95" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I95">
         <v>63.23</v>
       </c>
       <c r="J95" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K95">
         <v>65.19</v>
       </c>
       <c r="L95" t="s">
-        <v>66</v>
+        <v>208</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.45">
@@ -4638,28 +4638,28 @@
         <v>19</v>
       </c>
       <c r="C96" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D96">
         <v>2024</v>
       </c>
       <c r="E96" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F96" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G96">
         <v>15</v>
       </c>
       <c r="H96" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I96">
         <v>57.7</v>
       </c>
       <c r="J96" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K96">
         <v>61.6</v>
@@ -4676,7 +4676,7 @@
         <v>22</v>
       </c>
       <c r="C97" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D97">
         <v>2022</v>
@@ -4685,25 +4685,25 @@
         <v>25</v>
       </c>
       <c r="F97" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G97">
         <v>32</v>
       </c>
       <c r="H97" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I97">
         <v>62.5</v>
       </c>
       <c r="J97" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K97">
         <v>60.18</v>
       </c>
       <c r="L97" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.45">
@@ -4714,7 +4714,7 @@
         <v>23</v>
       </c>
       <c r="C98" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D98">
         <v>2023</v>
@@ -4723,25 +4723,25 @@
         <v>64</v>
       </c>
       <c r="F98" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G98">
         <v>40</v>
       </c>
       <c r="H98" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I98">
         <v>98.39</v>
       </c>
       <c r="J98" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K98">
         <v>99.19</v>
       </c>
       <c r="L98" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.45">
@@ -4752,7 +4752,7 @@
         <v>24</v>
       </c>
       <c r="C99" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D99">
         <v>2024</v>
@@ -4761,25 +4761,25 @@
         <v>64</v>
       </c>
       <c r="F99" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G99">
         <v>40</v>
       </c>
       <c r="H99" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I99">
         <v>86.15</v>
       </c>
       <c r="J99" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K99">
         <v>85.8</v>
       </c>
       <c r="L99" t="s">
-        <v>66</v>
+        <v>208</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.45">
@@ -4790,34 +4790,34 @@
         <v>25</v>
       </c>
       <c r="C100" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D100">
         <v>2022</v>
       </c>
       <c r="E100" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F100" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G100">
         <v>40</v>
       </c>
       <c r="H100" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I100">
         <v>58.3</v>
       </c>
       <c r="J100" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K100">
         <v>55.600000000000009</v>
       </c>
       <c r="L100" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.45">
@@ -4828,28 +4828,28 @@
         <v>26</v>
       </c>
       <c r="C101" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D101">
         <v>2022</v>
       </c>
       <c r="E101" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F101" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G101">
         <v>40</v>
       </c>
       <c r="H101" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I101">
         <v>58.5</v>
       </c>
       <c r="J101" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K101">
         <v>55.3</v>
@@ -4866,28 +4866,28 @@
         <v>27</v>
       </c>
       <c r="C102" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D102">
         <v>2022</v>
       </c>
       <c r="E102" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F102" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G102">
         <v>40</v>
       </c>
       <c r="H102" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I102">
         <v>56.3</v>
       </c>
       <c r="J102" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K102">
         <v>54.6</v>
@@ -4904,34 +4904,34 @@
         <v>28</v>
       </c>
       <c r="C103" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D103">
         <v>2022</v>
       </c>
       <c r="E103" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F103" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G103">
         <v>40</v>
       </c>
       <c r="H103" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I103">
         <v>54.3</v>
       </c>
       <c r="J103" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K103">
         <v>53.6</v>
       </c>
       <c r="L103" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.45">
@@ -4942,34 +4942,34 @@
         <v>29</v>
       </c>
       <c r="C104" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D104">
         <v>2024</v>
       </c>
       <c r="E104" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F104" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G104">
         <v>80</v>
       </c>
       <c r="H104" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I104">
         <v>76.649999999999991</v>
       </c>
       <c r="J104" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K104">
         <v>80.210000000000008</v>
       </c>
       <c r="L104" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.45">
@@ -4980,34 +4980,34 @@
         <v>30</v>
       </c>
       <c r="C105" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D105">
         <v>2024</v>
       </c>
       <c r="E105" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F105" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G105">
         <v>80</v>
       </c>
       <c r="H105" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I105">
         <v>74.760000000000005</v>
       </c>
       <c r="J105" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K105">
         <v>76.709999999999994</v>
       </c>
       <c r="L105" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.45">
@@ -5018,28 +5018,28 @@
         <v>31</v>
       </c>
       <c r="C106" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D106">
         <v>2024</v>
       </c>
       <c r="E106" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F106" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G106">
         <v>80</v>
       </c>
       <c r="H106" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I106">
         <v>73.790000000000006</v>
       </c>
       <c r="J106" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K106">
         <v>70.95</v>
@@ -5056,28 +5056,28 @@
         <v>32</v>
       </c>
       <c r="C107" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D107">
         <v>2024</v>
       </c>
       <c r="E107" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F107" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G107">
         <v>80</v>
       </c>
       <c r="H107" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I107">
         <v>73.27</v>
       </c>
       <c r="J107" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K107">
         <v>74.92</v>
@@ -5094,28 +5094,28 @@
         <v>33</v>
       </c>
       <c r="C108" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D108">
         <v>2024</v>
       </c>
       <c r="E108" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F108" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G108">
         <v>80</v>
       </c>
       <c r="H108" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I108">
         <v>73.98</v>
       </c>
       <c r="J108" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K108">
         <v>75.84</v>
@@ -5132,28 +5132,28 @@
         <v>34</v>
       </c>
       <c r="C109" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D109">
         <v>2022</v>
       </c>
       <c r="E109" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F109" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G109">
         <v>32</v>
       </c>
       <c r="H109" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I109">
         <v>63.3</v>
       </c>
       <c r="J109" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K109">
         <v>65.2</v>
@@ -5170,34 +5170,34 @@
         <v>35</v>
       </c>
       <c r="C110" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D110">
         <v>2022</v>
       </c>
       <c r="E110" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F110" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G110">
         <v>32</v>
       </c>
       <c r="H110" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I110">
         <v>74.5</v>
       </c>
       <c r="J110" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K110">
         <v>76.3</v>
       </c>
       <c r="L110" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.45">
@@ -5208,28 +5208,28 @@
         <v>36</v>
       </c>
       <c r="C111" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D111">
         <v>2022</v>
       </c>
       <c r="E111" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F111" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G111">
         <v>32</v>
       </c>
       <c r="H111" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I111">
         <v>74.5</v>
       </c>
       <c r="J111" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K111">
         <v>77.8</v>
@@ -5246,34 +5246,34 @@
         <v>37</v>
       </c>
       <c r="C112" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D112">
         <v>2022</v>
       </c>
       <c r="E112" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F112" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G112">
         <v>32</v>
       </c>
       <c r="H112" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I112">
         <v>67.800000000000011</v>
       </c>
       <c r="J112" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K112">
         <v>69</v>
       </c>
       <c r="L112" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.45">
@@ -5284,34 +5284,34 @@
         <v>38</v>
       </c>
       <c r="C113" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D113">
         <v>2022</v>
       </c>
       <c r="E113" t="s">
+        <v>186</v>
+      </c>
+      <c r="F113" t="s">
         <v>187</v>
       </c>
-      <c r="F113" t="s">
-        <v>188</v>
-      </c>
       <c r="G113">
         <v>32</v>
       </c>
       <c r="H113" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I113">
         <v>74.400000000000006</v>
       </c>
       <c r="J113" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K113">
         <v>82.8</v>
       </c>
       <c r="L113" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.45">
@@ -5322,7 +5322,7 @@
         <v>39</v>
       </c>
       <c r="C114" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D114">
         <v>2022</v>
@@ -5331,19 +5331,19 @@
         <v>25</v>
       </c>
       <c r="F114" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G114">
         <v>32</v>
       </c>
       <c r="H114" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I114">
         <v>69</v>
       </c>
       <c r="J114" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K114">
         <v>77</v>
@@ -5360,7 +5360,7 @@
         <v>40</v>
       </c>
       <c r="C115" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D115">
         <v>2022</v>
@@ -5369,25 +5369,25 @@
         <v>25</v>
       </c>
       <c r="F115" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G115">
         <v>32</v>
       </c>
       <c r="H115" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I115">
         <v>73.400000000000006</v>
       </c>
       <c r="J115" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K115">
         <v>71.399999999999991</v>
       </c>
       <c r="L115" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.45">
@@ -5398,7 +5398,7 @@
         <v>41</v>
       </c>
       <c r="C116" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D116">
         <v>2022</v>
@@ -5407,19 +5407,19 @@
         <v>25</v>
       </c>
       <c r="F116" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G116">
         <v>32</v>
       </c>
       <c r="H116" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I116">
         <v>71.399999999999991</v>
       </c>
       <c r="J116" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K116">
         <v>73.3</v>
@@ -5436,7 +5436,7 @@
         <v>42</v>
       </c>
       <c r="C117" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D117">
         <v>2022</v>
@@ -5445,25 +5445,25 @@
         <v>25</v>
       </c>
       <c r="F117" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G117">
         <v>32</v>
       </c>
       <c r="H117" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I117">
         <v>69.099999999999994</v>
       </c>
       <c r="J117" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K117">
         <v>68</v>
       </c>
       <c r="L117" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.45">
@@ -5474,7 +5474,7 @@
         <v>43</v>
       </c>
       <c r="C118" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D118">
         <v>2022</v>
@@ -5483,25 +5483,25 @@
         <v>25</v>
       </c>
       <c r="F118" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G118">
         <v>32</v>
       </c>
       <c r="H118" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I118">
         <v>80.2</v>
       </c>
       <c r="J118" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K118">
         <v>79.3</v>
       </c>
       <c r="L118" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.45">
@@ -5512,7 +5512,7 @@
         <v>44</v>
       </c>
       <c r="C119" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D119">
         <v>2023</v>
@@ -5521,25 +5521,25 @@
         <v>64</v>
       </c>
       <c r="F119" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G119">
         <v>40</v>
       </c>
       <c r="H119" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I119">
         <v>83</v>
       </c>
       <c r="J119" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K119">
         <v>81</v>
       </c>
       <c r="L119" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.45">
@@ -5550,7 +5550,7 @@
         <v>45</v>
       </c>
       <c r="C120" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D120">
         <v>2022</v>
@@ -5559,25 +5559,25 @@
         <v>64</v>
       </c>
       <c r="F120" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G120">
         <v>32</v>
       </c>
       <c r="H120" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I120">
         <v>83.42</v>
       </c>
       <c r="J120" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K120">
         <v>77.149999999999991</v>
       </c>
       <c r="L120" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.45">
@@ -5588,7 +5588,7 @@
         <v>46</v>
       </c>
       <c r="C121" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D121">
         <v>2022</v>
@@ -5597,25 +5597,25 @@
         <v>64</v>
       </c>
       <c r="F121" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G121">
         <v>32</v>
       </c>
       <c r="H121" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I121">
         <v>78.2</v>
       </c>
       <c r="J121" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K121">
         <v>75.87</v>
       </c>
       <c r="L121" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.45">
@@ -5626,7 +5626,7 @@
         <v>47</v>
       </c>
       <c r="C122" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D122">
         <v>2022</v>
@@ -5635,19 +5635,19 @@
         <v>64</v>
       </c>
       <c r="F122" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G122">
         <v>32</v>
       </c>
       <c r="H122" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I122">
         <v>60.95</v>
       </c>
       <c r="J122" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K122">
         <v>59.7</v>
@@ -5664,7 +5664,7 @@
         <v>48</v>
       </c>
       <c r="C123" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D123">
         <v>2022</v>
@@ -5673,25 +5673,25 @@
         <v>64</v>
       </c>
       <c r="F123" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G123">
         <v>32</v>
       </c>
       <c r="H123" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I123">
         <v>65.19</v>
       </c>
       <c r="J123" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K123">
         <v>64.52</v>
       </c>
       <c r="L123" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.45">
@@ -5702,34 +5702,34 @@
         <v>49</v>
       </c>
       <c r="C124" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D124">
         <v>2024</v>
       </c>
       <c r="E124" t="s">
+        <v>191</v>
+      </c>
+      <c r="F124" t="s">
         <v>192</v>
-      </c>
-      <c r="F124" t="s">
-        <v>193</v>
       </c>
       <c r="G124">
         <v>34</v>
       </c>
       <c r="H124" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I124">
         <v>91.490000000000009</v>
       </c>
       <c r="J124" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K124">
         <v>63.83</v>
       </c>
       <c r="L124" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.45">
@@ -5740,34 +5740,34 @@
         <v>50</v>
       </c>
       <c r="C125" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D125">
         <v>2024</v>
       </c>
       <c r="E125" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F125" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G125">
         <v>34</v>
       </c>
       <c r="H125" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I125">
         <v>82.98</v>
       </c>
       <c r="J125" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K125">
         <v>56.38</v>
       </c>
       <c r="L125" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.45">
@@ -5778,34 +5778,34 @@
         <v>51</v>
       </c>
       <c r="C126" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D126">
         <v>2024</v>
       </c>
       <c r="E126" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F126" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G126">
         <v>34</v>
       </c>
       <c r="H126" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I126">
         <v>61.7</v>
       </c>
       <c r="J126" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K126">
         <v>56.38</v>
       </c>
       <c r="L126" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.45">
@@ -5816,28 +5816,28 @@
         <v>52</v>
       </c>
       <c r="C127" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D127">
         <v>2024</v>
       </c>
       <c r="E127" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F127" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G127">
         <v>34</v>
       </c>
       <c r="H127" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I127">
         <v>86.89</v>
       </c>
       <c r="J127" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K127">
         <v>74.660000000000011</v>
@@ -5854,28 +5854,28 @@
         <v>53</v>
       </c>
       <c r="C128" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D128">
         <v>2024</v>
       </c>
       <c r="E128" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F128" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G128">
         <v>34</v>
       </c>
       <c r="H128" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I128">
         <v>87.5</v>
       </c>
       <c r="J128" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K128">
         <v>56.25</v>
@@ -5892,34 +5892,34 @@
         <v>54</v>
       </c>
       <c r="C129" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D129">
         <v>2024</v>
       </c>
       <c r="E129" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F129" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G129">
         <v>34</v>
       </c>
       <c r="H129" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I129">
         <v>92.320000000000007</v>
       </c>
       <c r="J129" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K129">
         <v>77.010000000000005</v>
       </c>
       <c r="L129" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.45">
@@ -5930,34 +5930,34 @@
         <v>55</v>
       </c>
       <c r="C130" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D130">
         <v>2021</v>
       </c>
       <c r="E130" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F130" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G130">
         <v>18</v>
       </c>
       <c r="H130" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I130">
         <v>55.55</v>
       </c>
       <c r="J130" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K130">
         <v>74.070000000000007</v>
       </c>
       <c r="L130" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.45">
@@ -5968,7 +5968,7 @@
         <v>56</v>
       </c>
       <c r="C131" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D131">
         <v>2024</v>
@@ -5977,19 +5977,19 @@
         <v>25</v>
       </c>
       <c r="F131" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G131">
         <v>32</v>
       </c>
       <c r="H131" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I131">
         <v>52.8</v>
       </c>
       <c r="J131" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K131">
         <v>53.7</v>
@@ -6006,7 +6006,7 @@
         <v>57</v>
       </c>
       <c r="C132" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D132">
         <v>2024</v>
@@ -6015,19 +6015,19 @@
         <v>25</v>
       </c>
       <c r="F132" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G132">
         <v>32</v>
       </c>
       <c r="H132" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I132">
         <v>57.499999999999993</v>
       </c>
       <c r="J132" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K132">
         <v>55.000000000000007</v>
@@ -6044,7 +6044,7 @@
         <v>58</v>
       </c>
       <c r="C133" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D133">
         <v>2024</v>
@@ -6053,25 +6053,25 @@
         <v>25</v>
       </c>
       <c r="F133" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G133">
         <v>32</v>
       </c>
       <c r="H133" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I133">
         <v>55.900000000000013</v>
       </c>
       <c r="J133" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K133">
         <v>54.500000000000007</v>
       </c>
       <c r="L133" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.45">
@@ -6082,7 +6082,7 @@
         <v>59</v>
       </c>
       <c r="C134" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D134">
         <v>2024</v>
@@ -6091,25 +6091,25 @@
         <v>25</v>
       </c>
       <c r="F134" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G134">
         <v>32</v>
       </c>
       <c r="H134" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I134">
         <v>52.7</v>
       </c>
       <c r="J134" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K134">
         <v>51.2</v>
       </c>
       <c r="L134" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.45">
@@ -6120,7 +6120,7 @@
         <v>60</v>
       </c>
       <c r="C135" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D135">
         <v>2021</v>
@@ -6129,19 +6129,19 @@
         <v>64</v>
       </c>
       <c r="F135" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G135">
         <v>40</v>
       </c>
       <c r="H135" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I135">
         <v>85.75</v>
       </c>
       <c r="J135" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K135">
         <v>84.5</v>
@@ -6158,28 +6158,28 @@
         <v>61</v>
       </c>
       <c r="C136" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D136">
         <v>2022</v>
       </c>
       <c r="E136" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F136" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G136">
         <v>58</v>
       </c>
       <c r="H136" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I136">
         <v>74.8</v>
       </c>
       <c r="J136" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K136">
         <v>76.900000000000006</v>
@@ -6196,28 +6196,28 @@
         <v>62</v>
       </c>
       <c r="C137" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D137">
         <v>2022</v>
       </c>
       <c r="E137" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F137" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G137">
         <v>58</v>
       </c>
       <c r="H137" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I137">
         <v>77.3</v>
       </c>
       <c r="J137" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K137">
         <v>80.5</v>
@@ -6234,34 +6234,34 @@
         <v>63</v>
       </c>
       <c r="C138" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D138">
         <v>2022</v>
       </c>
       <c r="E138" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F138" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G138">
         <v>58</v>
       </c>
       <c r="H138" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I138">
         <v>71.5</v>
       </c>
       <c r="J138" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K138">
         <v>76.099999999999994</v>
       </c>
       <c r="L138" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.45">
@@ -6272,34 +6272,34 @@
         <v>64</v>
       </c>
       <c r="C139" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D139">
         <v>2022</v>
       </c>
       <c r="E139" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F139" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G139">
         <v>58</v>
       </c>
       <c r="H139" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I139">
         <v>62.3</v>
       </c>
       <c r="J139" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K139">
         <v>60.099999999999987</v>
       </c>
       <c r="L139" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.45">
@@ -6310,34 +6310,34 @@
         <v>65</v>
       </c>
       <c r="C140" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D140">
         <v>2022</v>
       </c>
       <c r="E140" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F140" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G140">
         <v>58</v>
       </c>
       <c r="H140" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I140">
         <v>61.4</v>
       </c>
       <c r="J140" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K140">
         <v>58.4</v>
       </c>
       <c r="L140" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.45">
@@ -6348,28 +6348,28 @@
         <v>66</v>
       </c>
       <c r="C141" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D141">
         <v>2021</v>
       </c>
       <c r="E141" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F141" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G141">
         <v>34</v>
       </c>
       <c r="H141" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I141">
         <v>87.5</v>
       </c>
       <c r="J141" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K141">
         <v>56.25</v>
@@ -6386,7 +6386,7 @@
         <v>67</v>
       </c>
       <c r="C142" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D142">
         <v>2023</v>
@@ -6395,19 +6395,19 @@
         <v>25</v>
       </c>
       <c r="F142" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G142">
         <v>32</v>
       </c>
       <c r="H142" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I142">
         <v>64.400000000000006</v>
       </c>
       <c r="J142" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K142">
         <v>65.100000000000009</v>
@@ -6424,7 +6424,7 @@
         <v>68</v>
       </c>
       <c r="C143" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D143">
         <v>2023</v>
@@ -6433,25 +6433,25 @@
         <v>25</v>
       </c>
       <c r="F143" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G143">
         <v>32</v>
       </c>
       <c r="H143" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I143">
         <v>60.2</v>
       </c>
       <c r="J143" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K143">
         <v>58.7</v>
       </c>
       <c r="L143" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.45">
@@ -6462,7 +6462,7 @@
         <v>69</v>
       </c>
       <c r="C144" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D144">
         <v>2023</v>
@@ -6471,19 +6471,19 @@
         <v>25</v>
       </c>
       <c r="F144" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G144">
         <v>32</v>
       </c>
       <c r="H144" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I144">
         <v>63.1</v>
       </c>
       <c r="J144" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K144">
         <v>64</v>
@@ -6500,7 +6500,7 @@
         <v>70</v>
       </c>
       <c r="C145" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D145">
         <v>2023</v>
@@ -6509,25 +6509,25 @@
         <v>14</v>
       </c>
       <c r="F145" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G145">
         <v>27</v>
       </c>
       <c r="H145" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I145">
         <v>60.5</v>
       </c>
       <c r="J145" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K145">
         <v>60.55</v>
       </c>
       <c r="L145" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.45">
@@ -6538,34 +6538,34 @@
         <v>71</v>
       </c>
       <c r="C146" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D146">
         <v>2024</v>
       </c>
       <c r="E146" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F146" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G146">
         <v>30</v>
       </c>
       <c r="H146" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I146">
         <v>67.31</v>
       </c>
       <c r="J146" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K146">
         <v>65.510000000000005</v>
       </c>
       <c r="L146" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.45">
@@ -6576,28 +6576,28 @@
         <v>72</v>
       </c>
       <c r="C147" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D147">
         <v>2024</v>
       </c>
       <c r="E147" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F147" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G147">
         <v>30</v>
       </c>
       <c r="H147" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I147">
         <v>79.790000000000006</v>
       </c>
       <c r="J147" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K147">
         <v>71.709999999999994</v>
@@ -6614,34 +6614,34 @@
         <v>73</v>
       </c>
       <c r="C148" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D148">
         <v>2024</v>
       </c>
       <c r="E148" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F148" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G148">
         <v>30</v>
       </c>
       <c r="H148" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I148">
         <v>78.149999999999991</v>
       </c>
       <c r="J148" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K148">
         <v>68.010000000000005</v>
       </c>
       <c r="L148" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.45">
@@ -6652,34 +6652,34 @@
         <v>74</v>
       </c>
       <c r="C149" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D149">
         <v>2024</v>
       </c>
       <c r="E149" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F149" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G149">
         <v>30</v>
       </c>
       <c r="H149" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I149">
         <v>69.98</v>
       </c>
       <c r="J149" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K149">
         <v>67.179999999999993</v>
       </c>
       <c r="L149" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.45">
@@ -6690,7 +6690,7 @@
         <v>75</v>
       </c>
       <c r="C150" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D150">
         <v>2023</v>
@@ -6699,25 +6699,25 @@
         <v>25</v>
       </c>
       <c r="F150" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G150">
         <v>32</v>
       </c>
       <c r="H150" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I150">
         <v>55.06</v>
       </c>
       <c r="J150" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K150">
         <v>69.179999999999993</v>
       </c>
       <c r="L150" t="s">
-        <v>66</v>
+        <v>208</v>
       </c>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.45">
@@ -6728,7 +6728,7 @@
         <v>76</v>
       </c>
       <c r="C151" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D151">
         <v>2023</v>
@@ -6737,25 +6737,25 @@
         <v>14</v>
       </c>
       <c r="F151" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G151">
         <v>32</v>
       </c>
       <c r="H151" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I151">
         <v>56.86</v>
       </c>
       <c r="J151" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K151">
         <v>59.56</v>
       </c>
       <c r="L151" t="s">
-        <v>66</v>
+        <v>208</v>
       </c>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.45">
@@ -6766,7 +6766,7 @@
         <v>77</v>
       </c>
       <c r="C152" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D152">
         <v>2021</v>
@@ -6775,25 +6775,25 @@
         <v>64</v>
       </c>
       <c r="F152" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G152">
         <v>32</v>
       </c>
       <c r="H152" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I152">
         <v>70</v>
       </c>
       <c r="J152" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K152">
         <v>71.099999999999994</v>
       </c>
       <c r="L152" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.45">
@@ -6804,7 +6804,7 @@
         <v>78</v>
       </c>
       <c r="C153" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D153">
         <v>2021</v>
@@ -6813,25 +6813,25 @@
         <v>64</v>
       </c>
       <c r="F153" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G153">
         <v>32</v>
       </c>
       <c r="H153" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I153">
         <v>79.100000000000009</v>
       </c>
       <c r="J153" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K153">
         <v>78.2</v>
       </c>
       <c r="L153" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.45">
@@ -6842,7 +6842,7 @@
         <v>79</v>
       </c>
       <c r="C154" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D154">
         <v>2021</v>
@@ -6851,25 +6851,25 @@
         <v>25</v>
       </c>
       <c r="F154" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G154">
         <v>32</v>
       </c>
       <c r="H154" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I154">
         <v>64.600000000000009</v>
       </c>
       <c r="J154" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K154">
         <v>65.3</v>
       </c>
       <c r="L154" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.45">
@@ -6880,7 +6880,7 @@
         <v>80</v>
       </c>
       <c r="C155" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D155">
         <v>2021</v>
@@ -6889,25 +6889,25 @@
         <v>25</v>
       </c>
       <c r="F155" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G155">
         <v>32</v>
       </c>
       <c r="H155" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I155">
         <v>69.199999999999989</v>
       </c>
       <c r="J155" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K155">
         <v>69.699999999999989</v>
       </c>
       <c r="L155" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>